<commit_message>
Adding the required columns required for the field report impact taxonomy
</commit_message>
<xml_diff>
--- a/RCode/MainlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/RCode/MainlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="136">
   <si>
     <t xml:space="preserve">src_orgtype</t>
   </si>
@@ -329,6 +329,105 @@
   </si>
   <si>
     <t xml:space="preserve">imptypaidallifrc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO-Field Reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_injured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_dead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_affected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_displaced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_assisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_localstaff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_volunteers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_expats_delegates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_potentially_affected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_highest_risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_num_injured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_num_dead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_num_missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_num_affected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_num_displaced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_num_assisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">health_min_num_assisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_num_potentially_affected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gov_num_highest_risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_num_injured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_num_dead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_num_missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_num_affected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_num_displaced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_num_assisted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_num_potentially_affected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_num_highest_risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dref_amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appeal_amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imminent_dref_amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forecast_based_action_amount</t>
   </si>
 </sst>
 </file>
@@ -565,10 +664,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1536,6 +1635,454 @@
         <v>102</v>
       </c>
     </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updating the country bounding box mapping/expansion routines
</commit_message>
<xml_diff>
--- a/RCode/MainlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/RCode/MainlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -307,7 +307,7 @@
     <t xml:space="preserve">IFRC</t>
   </si>
   <si>
-    <t xml:space="preserve">GO-Appeal</t>
+    <t xml:space="preserve">GO-App</t>
   </si>
   <si>
     <t xml:space="preserve">num_beneficiaries</t>
@@ -331,7 +331,7 @@
     <t xml:space="preserve">imptypaidallifrc</t>
   </si>
   <si>
-    <t xml:space="preserve">GO-Field Reports</t>
+    <t xml:space="preserve">GO-FR</t>
   </si>
   <si>
     <t xml:space="preserve">num_injured</t>
@@ -564,12 +564,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -635,24 +635,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,7 +1559,7 @@
       <c r="B32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1588,7 +1588,7 @@
       <c r="B33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -2191,7 +2191,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Changing from two tables: impact & hazard, to one
</commit_message>
<xml_diff>
--- a/RCode/MainlyImpactData/ConvertImpact_Taxonomy.xlsx
+++ b/RCode/MainlyImpactData/ConvertImpact_Taxonomy.xlsx
@@ -43,13 +43,13 @@
     <t xml:space="preserve">impactdetails</t>
   </si>
   <si>
-    <t xml:space="preserve">measunits</t>
+    <t xml:space="preserve">imp_units</t>
   </si>
   <si>
     <t xml:space="preserve">imptype</t>
   </si>
   <si>
-    <t xml:space="preserve">impmethod</t>
+    <t xml:space="preserve">est_type</t>
   </si>
   <si>
     <t xml:space="preserve">orgtypeun</t>
@@ -659,8 +659,8 @@
   </sheetPr>
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>